<commit_message>
Updated inbreeding test data for mixed modelling in sommer v4.04
</commit_message>
<xml_diff>
--- a/inbreedtestdata.xlsx
+++ b/inbreedtestdata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elroy/Documents/University/Honours 2019/Everything/Data Analysis/Mixed Model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elroy/Documents/University/Honours 2019/Everything/BIOINFOMATICS/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="1200" windowWidth="21660" windowHeight="15760" tabRatio="500"/>
+    <workbookView xWindow="1840" yWindow="1160" windowWidth="21660" windowHeight="15760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="129">
   <si>
     <t>A37114</t>
   </si>
@@ -415,16 +415,13 @@
   </si>
   <si>
     <t>ID</t>
-  </si>
-  <si>
-    <t>Distance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -494,13 +491,6 @@
       <color rgb="FF333333"/>
       <name val="Lucida Grande"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -522,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -556,7 +546,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -834,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H114"/>
+  <dimension ref="A1:G114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -848,7 +837,7 @@
     <col min="8" max="16384" width="14.33203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>128</v>
       </c>
@@ -870,11 +859,8 @@
       <c r="G1" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -894,11 +880,8 @@
       <c r="G2" s="10">
         <v>0.12558908999999999</v>
       </c>
-      <c r="H2" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -918,11 +901,8 @@
       <c r="G3" s="10">
         <v>0.19224501999999999</v>
       </c>
-      <c r="H3" s="13">
-        <v>1166682.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -942,11 +922,8 @@
       <c r="G4" s="10">
         <v>0.13135716</v>
       </c>
-      <c r="H4" s="13">
-        <v>356917.9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -966,11 +943,8 @@
       <c r="G5" s="10">
         <v>0.1188192</v>
       </c>
-      <c r="H5" s="13">
-        <v>356917.9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
@@ -990,11 +964,8 @@
       <c r="G6" s="10">
         <v>0.37466045999999997</v>
       </c>
-      <c r="H6" s="13">
-        <v>701478.3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>5</v>
       </c>
@@ -1014,11 +985,8 @@
       <c r="G7" s="10">
         <v>0.13073272999999999</v>
       </c>
-      <c r="H7" s="13">
-        <v>2346794.2999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>6</v>
       </c>
@@ -1038,11 +1006,8 @@
       <c r="G8" s="10">
         <v>0.12784421000000001</v>
       </c>
-      <c r="H8" s="13">
-        <v>1827588.7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
@@ -1062,11 +1027,8 @@
       <c r="G9" s="10">
         <v>0.12168428000000001</v>
       </c>
-      <c r="H9" s="13">
-        <v>2346794.2999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>8</v>
       </c>
@@ -1086,11 +1048,8 @@
       <c r="G10" s="10">
         <v>0.13076752</v>
       </c>
-      <c r="H10" s="13">
-        <v>2119629.2000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>9</v>
       </c>
@@ -1110,11 +1069,8 @@
       <c r="G11" s="10">
         <v>0.25736827000000001</v>
       </c>
-      <c r="H11" s="13">
-        <v>1472116.7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
@@ -1134,11 +1090,8 @@
       <c r="G12" s="10">
         <v>8.8742070000000006E-2</v>
       </c>
-      <c r="H12" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>11</v>
       </c>
@@ -1160,11 +1113,8 @@
       <c r="G13" s="10">
         <v>0.38815808000000002</v>
       </c>
-      <c r="H13" s="13">
-        <v>2346496.4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>12</v>
       </c>
@@ -1186,11 +1136,8 @@
       <c r="G14" s="10">
         <v>0.25502095000000002</v>
       </c>
-      <c r="H14" s="13">
-        <v>2345803.4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>13</v>
       </c>
@@ -1210,11 +1157,8 @@
       <c r="G15" s="10">
         <v>0.12864323</v>
       </c>
-      <c r="H15" s="13">
-        <v>2346794.2999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>14</v>
       </c>
@@ -1234,11 +1178,8 @@
       <c r="G16" s="10">
         <v>0.13128711000000001</v>
       </c>
-      <c r="H16" s="13">
-        <v>2346794.2999999998</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>15</v>
       </c>
@@ -1258,11 +1199,8 @@
       <c r="G17" s="10">
         <v>0.18956006</v>
       </c>
-      <c r="H17" s="13">
-        <v>2346794.2999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>16</v>
       </c>
@@ -1282,11 +1220,8 @@
       <c r="G18" s="10">
         <v>9.4127970000000005E-2</v>
       </c>
-      <c r="H18" s="13">
-        <v>2346794.2999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>17</v>
       </c>
@@ -1308,11 +1243,8 @@
       <c r="G19" s="10">
         <v>9.483055E-2</v>
       </c>
-      <c r="H19" s="13">
-        <v>1668308.1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>18</v>
       </c>
@@ -1334,11 +1266,8 @@
       <c r="G20" s="10">
         <v>9.6312809999999999E-2</v>
       </c>
-      <c r="H20" s="13">
-        <v>1668296.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>19</v>
       </c>
@@ -1360,11 +1289,8 @@
       <c r="G21" s="10">
         <v>0.12530832</v>
       </c>
-      <c r="H21" s="13">
-        <v>1668273.3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>20</v>
       </c>
@@ -1386,11 +1312,8 @@
       <c r="G22" s="10">
         <v>0.10074149</v>
       </c>
-      <c r="H22" s="13">
-        <v>1668261.7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>21</v>
       </c>
@@ -1410,11 +1333,8 @@
       <c r="G23" s="10">
         <v>8.9608289999999993E-2</v>
       </c>
-      <c r="H23" s="13">
-        <v>1326166.1000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>22</v>
       </c>
@@ -1436,11 +1356,8 @@
       <c r="G24" s="10">
         <v>9.8226019999999997E-2</v>
       </c>
-      <c r="H24" s="13">
-        <v>1911994</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>23</v>
       </c>
@@ -1462,11 +1379,8 @@
       <c r="G25" s="10">
         <v>0.12666239000000001</v>
       </c>
-      <c r="H25" s="13">
-        <v>1932972.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>24</v>
       </c>
@@ -1488,11 +1402,8 @@
       <c r="G26" s="10">
         <v>9.9784310000000001E-2</v>
       </c>
-      <c r="H26" s="13">
-        <v>1851082.2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>25</v>
       </c>
@@ -1514,11 +1425,8 @@
       <c r="G27" s="10">
         <v>0.10056274</v>
       </c>
-      <c r="H27" s="13">
-        <v>1887230</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>26</v>
       </c>
@@ -1538,11 +1446,8 @@
       <c r="G28" s="10">
         <v>0.19190225</v>
       </c>
-      <c r="H28" s="13">
-        <v>575959.69999999995</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>27</v>
       </c>
@@ -1564,11 +1469,8 @@
       <c r="G29" s="10">
         <v>0.37015357999999998</v>
       </c>
-      <c r="H29" s="13">
-        <v>2200271.7999999998</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>28</v>
       </c>
@@ -1590,11 +1492,8 @@
       <c r="G30" s="10">
         <v>0.19076083999999999</v>
       </c>
-      <c r="H30" s="13">
-        <v>2206831.2999999998</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>29</v>
       </c>
@@ -1616,11 +1515,8 @@
       <c r="G31" s="10">
         <v>9.8872420000000003E-2</v>
       </c>
-      <c r="H31" s="13">
-        <v>2704997.1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>30</v>
       </c>
@@ -1642,11 +1538,8 @@
       <c r="G32" s="10">
         <v>0.12406892</v>
       </c>
-      <c r="H32" s="13">
-        <v>1932972.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>31</v>
       </c>
@@ -1668,11 +1561,8 @@
       <c r="G33" s="10">
         <v>8.8444430000000004E-2</v>
       </c>
-      <c r="H33" s="13">
-        <v>887932</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>32</v>
       </c>
@@ -1694,11 +1584,8 @@
       <c r="G34" s="10">
         <v>0.17632900000000001</v>
       </c>
-      <c r="H34" s="13">
-        <v>1903632.4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
         <v>33</v>
       </c>
@@ -1720,11 +1607,8 @@
       <c r="G35" s="10">
         <v>9.9653900000000004E-2</v>
       </c>
-      <c r="H35" s="13">
-        <v>1030714.5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>34</v>
       </c>
@@ -1746,11 +1630,8 @@
       <c r="G36" s="10">
         <v>9.9677429999999997E-2</v>
       </c>
-      <c r="H36" s="13">
-        <v>1086716.6000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
         <v>35</v>
       </c>
@@ -1772,11 +1653,8 @@
       <c r="G37" s="10">
         <v>0.49589433999999999</v>
       </c>
-      <c r="H37" s="13">
-        <v>1102176.1000000001</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>36</v>
       </c>
@@ -1798,11 +1676,8 @@
       <c r="G38" s="10">
         <v>9.5311019999999996E-2</v>
       </c>
-      <c r="H38" s="13">
-        <v>923218.4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
         <v>37</v>
       </c>
@@ -1822,11 +1697,8 @@
       <c r="G39" s="10">
         <v>0.19467406000000001</v>
       </c>
-      <c r="H39" s="13">
-        <v>1428038.9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
         <v>38</v>
       </c>
@@ -1848,11 +1720,8 @@
       <c r="G40" s="10">
         <v>0.1238783</v>
       </c>
-      <c r="H40" s="13">
-        <v>1093210.8999999999</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>39</v>
       </c>
@@ -1874,11 +1743,8 @@
       <c r="G41" s="10">
         <v>0.12691192000000001</v>
       </c>
-      <c r="H41" s="13">
-        <v>3165720.1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
         <v>40</v>
       </c>
@@ -1900,11 +1766,8 @@
       <c r="G42" s="10">
         <v>0.17956406999999999</v>
       </c>
-      <c r="H42" s="13">
-        <v>1837466.8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>41</v>
       </c>
@@ -1926,11 +1789,8 @@
       <c r="G43" s="10">
         <v>0.18702962000000001</v>
       </c>
-      <c r="H43" s="13">
-        <v>2423385.7999999998</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
         <v>42</v>
       </c>
@@ -1952,11 +1812,8 @@
       <c r="G44" s="10">
         <v>9.5734780000000005E-2</v>
       </c>
-      <c r="H44" s="13">
-        <v>2187151.7000000002</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
         <v>43</v>
       </c>
@@ -1978,11 +1835,8 @@
       <c r="G45" s="10">
         <v>0.37522253</v>
       </c>
-      <c r="H45" s="13">
-        <v>892726.7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
         <v>44</v>
       </c>
@@ -2004,11 +1858,8 @@
       <c r="G46" s="10">
         <v>0.36369422000000001</v>
       </c>
-      <c r="H46" s="13">
-        <v>887932</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="12" t="s">
         <v>45</v>
       </c>
@@ -2030,11 +1881,8 @@
       <c r="G47" s="10">
         <v>0.12594672000000001</v>
       </c>
-      <c r="H47" s="13">
-        <v>2345803.4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="12" t="s">
         <v>46</v>
       </c>
@@ -2056,11 +1904,8 @@
       <c r="G48" s="10">
         <v>0.13944943000000001</v>
       </c>
-      <c r="H48" s="13">
-        <v>913909.6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="12" t="s">
         <v>47</v>
       </c>
@@ -2082,11 +1927,8 @@
       <c r="G49" s="10">
         <v>0.12801309999999999</v>
       </c>
-      <c r="H49" s="13">
-        <v>149170.1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="12" t="s">
         <v>48</v>
       </c>
@@ -2108,11 +1950,8 @@
       <c r="G50" s="10">
         <v>9.3225749999999996E-2</v>
       </c>
-      <c r="H50" s="13">
-        <v>892726.7</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="12" t="s">
         <v>49</v>
       </c>
@@ -2134,11 +1973,8 @@
       <c r="G51" s="10">
         <v>0.12836470999999999</v>
       </c>
-      <c r="H51" s="13">
-        <v>2140808.7999999998</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="12" t="s">
         <v>50</v>
       </c>
@@ -2160,11 +1996,8 @@
       <c r="G52" s="10">
         <v>9.9645410000000004E-2</v>
       </c>
-      <c r="H52" s="13">
-        <v>2943805.2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="12" t="s">
         <v>51</v>
       </c>
@@ -2186,11 +2019,8 @@
       <c r="G53" s="10">
         <v>0.27824366</v>
       </c>
-      <c r="H53" s="13">
-        <v>2346794.2999999998</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="12" t="s">
         <v>52</v>
       </c>
@@ -2212,11 +2042,8 @@
       <c r="G54" s="10">
         <v>0.10018982999999999</v>
       </c>
-      <c r="H54" s="13">
-        <v>2225249</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="12" t="s">
         <v>53</v>
       </c>
@@ -2236,11 +2063,8 @@
       <c r="G55" s="10">
         <v>0.19838569</v>
       </c>
-      <c r="H55" s="13">
-        <v>1479097.7</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="12" t="s">
         <v>54</v>
       </c>
@@ -2262,11 +2086,8 @@
       <c r="G56" s="10">
         <v>0.12548098999999999</v>
       </c>
-      <c r="H56" s="13">
-        <v>2181718</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="12" t="s">
         <v>55</v>
       </c>
@@ -2288,11 +2109,8 @@
       <c r="G57" s="10">
         <v>0.12871915</v>
       </c>
-      <c r="H57" s="13">
-        <v>2059640.8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="12" t="s">
         <v>56</v>
       </c>
@@ -2314,11 +2132,8 @@
       <c r="G58" s="10">
         <v>0.13024583000000001</v>
       </c>
-      <c r="H58" s="13">
-        <v>1745506.2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="12" t="s">
         <v>57</v>
       </c>
@@ -2340,11 +2155,8 @@
       <c r="G59" s="10">
         <v>0.11977354</v>
       </c>
-      <c r="H59" s="13">
-        <v>2883845.1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="12" t="s">
         <v>58</v>
       </c>
@@ -2366,11 +2178,8 @@
       <c r="G60" s="10">
         <v>0.10000011</v>
       </c>
-      <c r="H60" s="13">
-        <v>3165720.1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="12" t="s">
         <v>59</v>
       </c>
@@ -2392,11 +2201,8 @@
       <c r="G61" s="10">
         <v>0.12469589</v>
       </c>
-      <c r="H61" s="13">
-        <v>2184030.2000000002</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="12" t="s">
         <v>60</v>
       </c>
@@ -2418,11 +2224,8 @@
       <c r="G62" s="10">
         <v>0.19249852000000001</v>
       </c>
-      <c r="H62" s="13">
-        <v>2296198.7000000002</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="12" t="s">
         <v>61</v>
       </c>
@@ -2444,11 +2247,8 @@
       <c r="G63" s="10">
         <v>0.12644482000000001</v>
       </c>
-      <c r="H63" s="13">
-        <v>1477037.1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="12" t="s">
         <v>62</v>
       </c>
@@ -2470,11 +2270,8 @@
       <c r="G64" s="10">
         <v>9.4081419999999999E-2</v>
       </c>
-      <c r="H64" s="13">
-        <v>921040.4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="12" t="s">
         <v>63</v>
       </c>
@@ -2496,11 +2293,8 @@
       <c r="G65" s="10">
         <v>9.3755980000000003E-2</v>
       </c>
-      <c r="H65" s="13">
-        <v>2778009.9</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="12" t="s">
         <v>64</v>
       </c>
@@ -2522,11 +2316,8 @@
       <c r="G66" s="10">
         <v>9.4070260000000003E-2</v>
       </c>
-      <c r="H66" s="13">
-        <v>2384948.1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="12" t="s">
         <v>65</v>
       </c>
@@ -2548,11 +2339,8 @@
       <c r="G67" s="10">
         <v>0.23942086000000001</v>
       </c>
-      <c r="H67" s="13">
-        <v>834472.1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="12" t="s">
         <v>66</v>
       </c>
@@ -2574,11 +2362,8 @@
       <c r="G68" s="10">
         <v>9.0403109999999995E-2</v>
       </c>
-      <c r="H68" s="13">
-        <v>2778009.9</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="12" t="s">
         <v>67</v>
       </c>
@@ -2600,11 +2385,8 @@
       <c r="G69" s="10">
         <v>8.9393769999999997E-2</v>
       </c>
-      <c r="H69" s="13">
-        <v>1174715.6000000001</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="12" t="s">
         <v>68</v>
       </c>
@@ -2624,11 +2406,8 @@
       <c r="G70" s="10">
         <v>9.3306780000000006E-2</v>
       </c>
-      <c r="H70" s="13">
-        <v>2346794.2999999998</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="12" t="s">
         <v>69</v>
       </c>
@@ -2650,11 +2429,8 @@
       <c r="G71" s="10">
         <v>0.12671721999999999</v>
       </c>
-      <c r="H71" s="13">
-        <v>2992392.5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="12" t="s">
         <v>70</v>
       </c>
@@ -2676,11 +2452,8 @@
       <c r="G72" s="10">
         <v>0.39839753999999999</v>
       </c>
-      <c r="H72" s="13">
-        <v>2406976.1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="12" t="s">
         <v>71</v>
       </c>
@@ -2702,11 +2475,8 @@
       <c r="G73" s="10">
         <v>9.1846730000000001E-2</v>
       </c>
-      <c r="H73" s="13">
-        <v>2496711.2000000002</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="12" t="s">
         <v>72</v>
       </c>
@@ -2728,11 +2498,8 @@
       <c r="G74" s="10">
         <v>0.37454757</v>
       </c>
-      <c r="H74" s="13">
-        <v>2059640.8</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="12" t="s">
         <v>73</v>
       </c>
@@ -2754,11 +2521,8 @@
       <c r="G75" s="10">
         <v>0.20015351000000001</v>
       </c>
-      <c r="H75" s="13">
-        <v>2274361.2999999998</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="12" t="s">
         <v>74</v>
       </c>
@@ -2780,11 +2544,8 @@
       <c r="G76" s="10">
         <v>9.3841099999999997E-2</v>
       </c>
-      <c r="H76" s="13">
-        <v>2496711.2000000002</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="12" t="s">
         <v>75</v>
       </c>
@@ -2806,11 +2567,8 @@
       <c r="G77" s="10">
         <v>0.18206705000000001</v>
       </c>
-      <c r="H77" s="13">
-        <v>2057538</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="12" t="s">
         <v>76</v>
       </c>
@@ -2832,11 +2590,8 @@
       <c r="G78" s="10">
         <v>0.49337047000000001</v>
       </c>
-      <c r="H78" s="13">
-        <v>1668284.9</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="12" t="s">
         <v>77</v>
       </c>
@@ -2858,11 +2613,8 @@
       <c r="G79" s="10">
         <v>9.0075219999999998E-2</v>
       </c>
-      <c r="H79" s="13">
-        <v>1899427.5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="12" t="s">
         <v>78</v>
       </c>
@@ -2884,11 +2636,8 @@
       <c r="G80" s="10">
         <v>0.18227710999999999</v>
       </c>
-      <c r="H80" s="13">
-        <v>1028746.1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="12" t="s">
         <v>79</v>
       </c>
@@ -2910,11 +2659,8 @@
       <c r="G81" s="10">
         <v>0.12723683999999999</v>
       </c>
-      <c r="H81" s="13">
-        <v>1899427.5</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="12" t="s">
         <v>80</v>
       </c>
@@ -2936,11 +2682,8 @@
       <c r="G82" s="10">
         <v>0.18428822</v>
       </c>
-      <c r="H82" s="13">
-        <v>941800.8</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="12" t="s">
         <v>81</v>
       </c>
@@ -2962,11 +2705,8 @@
       <c r="G83" s="10">
         <v>0.12378978</v>
       </c>
-      <c r="H83" s="13">
-        <v>2501091.9</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="12" t="s">
         <v>82</v>
       </c>
@@ -2988,11 +2728,8 @@
       <c r="G84" s="10">
         <v>0.13125929</v>
       </c>
-      <c r="H84" s="13">
-        <v>773589.1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="12" t="s">
         <v>83</v>
       </c>
@@ -3014,11 +2751,8 @@
       <c r="G85" s="10">
         <v>0.12202223</v>
       </c>
-      <c r="H85" s="13">
-        <v>1208004.3999999999</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="12" t="s">
         <v>84</v>
       </c>
@@ -3040,11 +2774,8 @@
       <c r="G86" s="10">
         <v>0.12254587</v>
       </c>
-      <c r="H86" s="13">
-        <v>1258868.2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="12" t="s">
         <v>85</v>
       </c>
@@ -3064,11 +2795,8 @@
       <c r="G87" s="10">
         <v>0.19277968000000001</v>
       </c>
-      <c r="H87" s="13">
-        <v>1332442.5</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="12" t="s">
         <v>86</v>
       </c>
@@ -3088,11 +2816,8 @@
       <c r="G88" s="10">
         <v>0.12199261</v>
       </c>
-      <c r="H88" s="13">
-        <v>941800.8</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="12" t="s">
         <v>87</v>
       </c>
@@ -3114,11 +2839,8 @@
       <c r="G89" s="10">
         <v>0.12498853</v>
       </c>
-      <c r="H89" s="13">
-        <v>943269.5</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="12" t="s">
         <v>88</v>
       </c>
@@ -3140,11 +2862,8 @@
       <c r="G90" s="10">
         <v>0.18839481</v>
       </c>
-      <c r="H90" s="13">
-        <v>1257685.3999999999</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="12" t="s">
         <v>89</v>
       </c>
@@ -3166,11 +2885,8 @@
       <c r="G91" s="10">
         <v>9.4501689999999999E-2</v>
       </c>
-      <c r="H91" s="13">
-        <v>941692.2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="12" t="s">
         <v>90</v>
       </c>
@@ -3192,11 +2908,8 @@
       <c r="G92" s="10">
         <v>0.18574777000000001</v>
       </c>
-      <c r="H92" s="13">
-        <v>1903632.4</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="12" t="s">
         <v>91</v>
       </c>
@@ -3218,11 +2931,8 @@
       <c r="G93" s="10">
         <v>0.18574372</v>
       </c>
-      <c r="H93" s="13">
-        <v>923218.4</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="12" t="s">
         <v>92</v>
       </c>
@@ -3244,11 +2954,8 @@
       <c r="G94" s="10">
         <v>9.7862299999999999E-2</v>
       </c>
-      <c r="H94" s="13">
-        <v>913909.6</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="12" t="s">
         <v>93</v>
       </c>
@@ -3268,11 +2975,8 @@
       <c r="G95" s="10">
         <v>0.19002200999999999</v>
       </c>
-      <c r="H95" s="13">
-        <v>1332605.3999999999</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="12" t="s">
         <v>94</v>
       </c>
@@ -3294,11 +2998,8 @@
       <c r="G96" s="10">
         <v>0.11933079000000001</v>
       </c>
-      <c r="H96" s="13">
-        <v>2680665.7999999998</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="12" t="s">
         <v>95</v>
       </c>
@@ -3320,11 +3021,8 @@
       <c r="G97" s="10">
         <v>0.49909713999999999</v>
       </c>
-      <c r="H97" s="13">
-        <v>922078.4</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="12" t="s">
         <v>96</v>
       </c>
@@ -3346,11 +3044,8 @@
       <c r="G98" s="10">
         <v>0.12355661</v>
       </c>
-      <c r="H98" s="13">
-        <v>1093210.8999999999</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="12" t="s">
         <v>97</v>
       </c>
@@ -3372,11 +3067,8 @@
       <c r="G99" s="10">
         <v>0.13979739999999999</v>
       </c>
-      <c r="H99" s="13">
-        <v>1900439.4</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="12" t="s">
         <v>98</v>
       </c>
@@ -3398,11 +3090,8 @@
       <c r="G100" s="10">
         <v>0.130605</v>
       </c>
-      <c r="H100" s="13">
-        <v>1073484.8999999999</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="12" t="s">
         <v>99</v>
       </c>
@@ -3424,11 +3113,8 @@
       <c r="G101" s="10">
         <v>0.12387902000000001</v>
       </c>
-      <c r="H101" s="13">
-        <v>1073484.8999999999</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="12" t="s">
         <v>100</v>
       </c>
@@ -3450,11 +3136,8 @@
       <c r="G102" s="10">
         <v>0.18210904</v>
       </c>
-      <c r="H102" s="13">
-        <v>3000537.6</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="12" t="s">
         <v>101</v>
       </c>
@@ -3476,11 +3159,8 @@
       <c r="G103" s="10">
         <v>0.19312871000000001</v>
       </c>
-      <c r="H103" s="13">
-        <v>2296198.7000000002</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="12" t="s">
         <v>102</v>
       </c>
@@ -3502,11 +3182,8 @@
       <c r="G104" s="10">
         <v>0.12542631000000001</v>
       </c>
-      <c r="H104" s="13">
-        <v>1641844.3</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="12" t="s">
         <v>103</v>
       </c>
@@ -3528,11 +3205,8 @@
       <c r="G105" s="10">
         <v>0.12622817</v>
       </c>
-      <c r="H105" s="13">
-        <v>1641844.3</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="12" t="s">
         <v>104</v>
       </c>
@@ -3554,11 +3228,8 @@
       <c r="G106" s="10">
         <v>8.9988620000000005E-2</v>
       </c>
-      <c r="H106" s="13">
-        <v>915619.5</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="12" t="s">
         <v>105</v>
       </c>
@@ -3580,11 +3251,8 @@
       <c r="G107" s="10">
         <v>0.18283395</v>
       </c>
-      <c r="H107" s="13">
-        <v>2274361.2999999998</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="12" t="s">
         <v>106</v>
       </c>
@@ -3606,11 +3274,8 @@
       <c r="G108" s="10">
         <v>0.25359156999999999</v>
       </c>
-      <c r="H108" s="13">
-        <v>589141.30000000005</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="12" t="s">
         <v>107</v>
       </c>
@@ -3632,11 +3297,8 @@
       <c r="G109" s="10">
         <v>8.894502E-2</v>
       </c>
-      <c r="H109" s="13">
-        <v>1215409</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="7" t="s">
         <v>108</v>
       </c>
@@ -3656,11 +3318,8 @@
       <c r="G110" s="10">
         <v>0.19041780999999999</v>
       </c>
-      <c r="H110" s="13">
-        <v>1166682.8</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="12" t="s">
         <v>109</v>
       </c>
@@ -3682,11 +3341,8 @@
       <c r="G111" s="10">
         <v>0.36605813999999998</v>
       </c>
-      <c r="H111" s="13">
-        <v>132364.6</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" s="12" t="s">
         <v>110</v>
       </c>
@@ -3706,11 +3362,8 @@
       <c r="G112" s="10">
         <v>0.19343558</v>
       </c>
-      <c r="H112" s="13">
-        <v>1308451</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" s="12" t="s">
         <v>111</v>
       </c>
@@ -3732,11 +3385,8 @@
       <c r="G113" s="10">
         <v>0.12026881</v>
       </c>
-      <c r="H113" s="13">
-        <v>1786033.1</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" s="12" t="s">
         <v>112</v>
       </c>
@@ -3757,9 +3407,6 @@
       </c>
       <c r="G114" s="10">
         <v>0.1246814</v>
-      </c>
-      <c r="H114" s="13">
-        <v>204273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>